<commit_message>
update des zones - correction d'erreurs
</commit_message>
<xml_diff>
--- a/inputlyrs/Fire.info/Zones_feux.xlsx
+++ b/inputlyrs/Fire.info/Zones_feux.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boumav\Desktop\QLD_V2\inputlyrs\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boumav\Desktop\QbcLDM\inputlyrs\Fire.info\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
   <si>
     <t>A</t>
   </si>
@@ -138,21 +138,9 @@
     <t>Récent: Analyse de la DIF basées sur la cartographie écoforestière, reflète environ 1930-2020</t>
   </si>
   <si>
-    <t>Moyen terme:études recensées dans les états de référence, basées sur des cartes de feux régionales, environ 1820-2010</t>
-  </si>
-  <si>
     <t>Z</t>
   </si>
   <si>
-    <t>OO</t>
-  </si>
-  <si>
-    <t>Fortement agricole, combustibles forestiers très épars - exclu des analyses pour l'instant</t>
-  </si>
-  <si>
-    <t>Partiellement agricole, combustibles forestiers épars - exclu des analyses pour l'instant</t>
-  </si>
-  <si>
     <t>Taille max (km2)</t>
   </si>
   <si>
@@ -162,13 +150,73 @@
     <t>Récent: Analyse de Erni et al. 2020 (données du fédéral 1970-2010)</t>
   </si>
   <si>
-    <t>vérifier</t>
-  </si>
-  <si>
     <t>Max200</t>
   </si>
   <si>
     <t>Max2000</t>
+  </si>
+  <si>
+    <t>urbain, agricole, combustibles forestiers épars - exclu des analyses pour l'instant</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Différence</t>
+  </si>
+  <si>
+    <t>Cycle, physiographie</t>
+  </si>
+  <si>
+    <t>Cycle</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Saisonalité</t>
+  </si>
+  <si>
+    <t>Types de combustibles, influence océanique</t>
+  </si>
+  <si>
+    <t>Cycle, taille des feux</t>
+  </si>
+  <si>
+    <t>Cycle, types de combustibles, taille des feux</t>
+  </si>
+  <si>
+    <t>Cycle (influence océanique)</t>
+  </si>
+  <si>
+    <t>Moyen terme:études recensées dans les états de référence, basées sur des cartes de feux régionales, environ 1820-2010 (Bouchard et al. 2015, Boucher et al. 2011)</t>
+  </si>
+  <si>
+    <t>agro-forestier, combustibles forestiers épars - exclu des analyses pour l'instant</t>
+  </si>
+  <si>
+    <t>Cycle, physiographie, types de combustibles (feuillu)</t>
+  </si>
+  <si>
+    <t>Centre</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>3389 (FRT1)</t>
+  </si>
+  <si>
+    <t>101 (FRT4)</t>
+  </si>
+  <si>
+    <t>364(FRT5)</t>
+  </si>
+  <si>
+    <t>3389(FRT1)</t>
+  </si>
+  <si>
+    <t>1030(FRT2)</t>
   </si>
 </sst>
 </file>
@@ -209,7 +257,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -217,131 +265,29 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -624,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,60 +588,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="20" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="20"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>42</v>
+      <c r="G2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="7">
         <v>250</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="16">
-        <v>7092.1985815602839</v>
-      </c>
-      <c r="G3" s="20">
+      <c r="F3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="9">
         <v>250</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="10" t="s">
         <v>33</v>
       </c>
     </row>
@@ -703,25 +651,25 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="7">
         <v>150</v>
       </c>
-      <c r="D4" s="15">
-        <v>100</v>
-      </c>
-      <c r="E4" s="15" t="s">
+      <c r="D4" s="7">
+        <v>150</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="16">
-        <v>100.8267795926598</v>
-      </c>
-      <c r="G4" s="20">
-        <v>150</v>
-      </c>
-      <c r="H4" s="20" t="s">
+      <c r="F4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="9">
+        <v>125</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>33</v>
       </c>
     </row>
@@ -729,25 +677,25 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="7">
+        <v>250</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="9">
         <v>200</v>
       </c>
-      <c r="E5" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="16">
-        <v>838.92617449664431</v>
-      </c>
-      <c r="G5" s="20">
-        <v>200</v>
-      </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="10" t="s">
         <v>33</v>
       </c>
     </row>
@@ -755,25 +703,25 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="7">
         <v>125</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="15" t="s">
+      <c r="D6" s="7">
+        <v>500</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="16">
-        <v>2347.4178403755868</v>
-      </c>
-      <c r="G6" s="20">
-        <v>350</v>
-      </c>
-      <c r="H6" s="20" t="s">
+      <c r="F6" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="9">
+        <v>300</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>34</v>
       </c>
     </row>
@@ -781,25 +729,25 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="7">
         <v>500</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="16">
-        <v>2347.4178403755868</v>
-      </c>
-      <c r="G7" s="20">
-        <v>500</v>
-      </c>
-      <c r="H7" s="20" t="s">
+      <c r="F7" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="9">
+        <v>750</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>34</v>
       </c>
     </row>
@@ -807,25 +755,25 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="7">
         <v>250</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="7">
         <v>400</v>
       </c>
-      <c r="F8" s="16">
-        <v>838.92617449664431</v>
-      </c>
-      <c r="G8" s="21">
+      <c r="F8" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="10">
         <v>250</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="10" t="s">
         <v>33</v>
       </c>
     </row>
@@ -833,66 +781,214 @@
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="19">
-        <v>7092.1985815602839</v>
-      </c>
-      <c r="G9" s="20">
-        <v>600</v>
-      </c>
-      <c r="H9" s="20" t="s">
+      <c r="F9" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="9">
+        <v>500</v>
+      </c>
+      <c r="H9" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>39</v>
+      <c r="A10" t="s">
+        <v>44</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="5"/>
+        <v>57</v>
+      </c>
+      <c r="C10" s="7">
+        <v>200</v>
+      </c>
+      <c r="D10" s="7">
+        <v>200</v>
+      </c>
+      <c r="E10" s="7">
+        <v>225</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="9">
+        <v>200</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>41</v>
+      <c r="A11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
+      <c r="B13" s="8"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24">
+        <f>100/0.27</f>
+        <v>370.37037037037032</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
         <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -922,26 +1018,26 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>4</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>3052</v>
       </c>
     </row>
@@ -949,10 +1045,10 @@
       <c r="A3">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>50</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>1119</v>
       </c>
       <c r="E3">
@@ -963,11 +1059,11 @@
         <f>C3</f>
         <v>1119</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="5">
         <f t="shared" ref="H3:I3" si="0">E3/E$36</f>
         <v>0.68231707317073176</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="5">
         <f t="shared" si="0"/>
         <v>0.65746180963572265</v>
       </c>
@@ -981,14 +1077,14 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <f>B4-50</f>
         <v>50</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>100</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>223</v>
       </c>
       <c r="E4">
@@ -999,11 +1095,11 @@
         <f t="shared" ref="F4:F30" si="2">C4</f>
         <v>223</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="5">
         <f t="shared" ref="H4:H31" si="3">E4/E$36</f>
         <v>0.13597560975609757</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="5">
         <f t="shared" ref="I4:I31" si="4">F4/F$36</f>
         <v>0.13102232667450059</v>
       </c>
@@ -1017,14 +1113,14 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <f t="shared" ref="A5:A35" si="7">B5-50</f>
         <v>100</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>150</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>116</v>
       </c>
       <c r="E5">
@@ -1035,11 +1131,11 @@
         <f t="shared" si="2"/>
         <v>116</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="5">
         <f t="shared" si="3"/>
         <v>7.0731707317073164E-2</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="5">
         <f t="shared" si="4"/>
         <v>6.8155111633372498E-2</v>
       </c>
@@ -1053,14 +1149,14 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <f t="shared" si="7"/>
         <v>150</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>200</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>63</v>
       </c>
       <c r="E6">
@@ -1071,11 +1167,11 @@
         <f t="shared" si="2"/>
         <v>63</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="5">
         <f t="shared" si="3"/>
         <v>3.8414634146341463E-2</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="5">
         <f t="shared" si="4"/>
         <v>3.7015276145710929E-2</v>
       </c>
@@ -1089,14 +1185,14 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <f t="shared" si="7"/>
         <v>200</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>250</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>30</v>
       </c>
       <c r="E7">
@@ -1107,11 +1203,11 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="5">
         <f t="shared" si="3"/>
         <v>1.8292682926829267E-2</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="5">
         <f t="shared" si="4"/>
         <v>1.7626321974148061E-2</v>
       </c>
@@ -1125,14 +1221,14 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <f t="shared" si="7"/>
         <v>250</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>300</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>29</v>
       </c>
       <c r="E8">
@@ -1143,11 +1239,11 @@
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="5">
         <f t="shared" si="3"/>
         <v>1.7682926829268291E-2</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="5">
         <f t="shared" si="4"/>
         <v>1.7038777908343124E-2</v>
       </c>
@@ -1161,14 +1257,14 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <f t="shared" si="7"/>
         <v>300</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>350</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>16</v>
       </c>
       <c r="E9">
@@ -1179,11 +1275,11 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="5">
         <f t="shared" si="3"/>
         <v>9.7560975609756097E-3</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="5">
         <f t="shared" si="4"/>
         <v>9.4007050528789656E-3</v>
       </c>
@@ -1197,14 +1293,14 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <f t="shared" si="7"/>
         <v>350</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>400</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>18</v>
       </c>
       <c r="E10">
@@ -1215,11 +1311,11 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="5">
         <f t="shared" si="3"/>
         <v>1.097560975609756E-2</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="5">
         <f t="shared" si="4"/>
         <v>1.0575793184488837E-2</v>
       </c>
@@ -1233,14 +1329,14 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <f t="shared" si="7"/>
         <v>400</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>450</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>17</v>
       </c>
       <c r="E11">
@@ -1251,11 +1347,11 @@
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="5">
         <f t="shared" si="3"/>
         <v>1.0365853658536586E-2</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="5">
         <f t="shared" si="4"/>
         <v>9.9882491186839006E-3</v>
       </c>
@@ -1269,14 +1365,14 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <f t="shared" si="7"/>
         <v>450</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>500</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>9</v>
       </c>
       <c r="E12">
@@ -1287,11 +1383,11 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="5">
         <f t="shared" si="3"/>
         <v>5.4878048780487802E-3</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="5">
         <f t="shared" si="4"/>
         <v>5.2878965922444187E-3</v>
       </c>
@@ -1305,25 +1401,25 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <f t="shared" si="7"/>
         <v>500</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>550</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>7</v>
       </c>
       <c r="F13">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="H13" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="7">
+      <c r="H13" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
         <f t="shared" si="4"/>
         <v>4.1128084606345478E-3</v>
       </c>
@@ -1337,25 +1433,25 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <f t="shared" si="7"/>
         <v>550</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>600</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>6</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="H14" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="7">
+      <c r="H14" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
         <f t="shared" si="4"/>
         <v>3.5252643948296123E-3</v>
       </c>
@@ -1369,25 +1465,25 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <f t="shared" si="7"/>
         <v>600</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>650</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>3</v>
       </c>
       <c r="F15">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H15" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="7">
+      <c r="H15" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
         <f t="shared" si="4"/>
         <v>1.7626321974148062E-3</v>
       </c>
@@ -1401,25 +1497,25 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <f t="shared" si="7"/>
         <v>650</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>700</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>2</v>
       </c>
       <c r="F16">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="H16" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="7">
+      <c r="H16" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
         <f t="shared" si="4"/>
         <v>1.1750881316098707E-3</v>
       </c>
@@ -1433,25 +1529,25 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <f t="shared" si="7"/>
         <v>700</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>750</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>5</v>
       </c>
       <c r="F17">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="H17" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="7">
+      <c r="H17" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
         <f t="shared" si="4"/>
         <v>2.9377203290246769E-3</v>
       </c>
@@ -1465,25 +1561,25 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <f t="shared" si="7"/>
         <v>750</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>800</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>4</v>
       </c>
       <c r="F18">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="H18" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="7">
+      <c r="H18" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
         <f t="shared" si="4"/>
         <v>2.3501762632197414E-3</v>
       </c>
@@ -1497,25 +1593,25 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <f t="shared" si="7"/>
         <v>800</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>850</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>3</v>
       </c>
       <c r="F19">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H19" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="7">
+      <c r="H19" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
         <f t="shared" si="4"/>
         <v>1.7626321974148062E-3</v>
       </c>
@@ -1529,25 +1625,25 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <f t="shared" si="7"/>
         <v>850</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>900</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>5</v>
       </c>
       <c r="F20">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="H20" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="7">
+      <c r="H20" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
         <f t="shared" si="4"/>
         <v>2.9377203290246769E-3</v>
       </c>
@@ -1561,25 +1657,25 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <f t="shared" si="7"/>
         <v>900</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>950</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>1</v>
       </c>
       <c r="F21">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H21" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="7">
+      <c r="H21" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
         <f t="shared" si="4"/>
         <v>5.8754406580493535E-4</v>
       </c>
@@ -1593,25 +1689,25 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <f t="shared" si="7"/>
         <v>950</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>1000</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>5</v>
       </c>
       <c r="F22">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="H22" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="7">
+      <c r="H22" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="5">
         <f t="shared" si="4"/>
         <v>2.9377203290246769E-3</v>
       </c>
@@ -1625,25 +1721,25 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <f t="shared" si="7"/>
         <v>1000</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>1050</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>1</v>
       </c>
       <c r="F23">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H23" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="7">
+      <c r="H23" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="5">
         <f t="shared" si="4"/>
         <v>5.8754406580493535E-4</v>
       </c>
@@ -1657,25 +1753,25 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <f t="shared" si="7"/>
         <v>1050</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>1100</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>3</v>
       </c>
       <c r="F24">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H24" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="7">
+      <c r="H24" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="5">
         <f t="shared" si="4"/>
         <v>1.7626321974148062E-3</v>
       </c>
@@ -1689,25 +1785,25 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <f t="shared" si="7"/>
         <v>1150</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>1200</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>2</v>
       </c>
       <c r="F25">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="H25" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="7">
+      <c r="H25" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="5">
         <f t="shared" si="4"/>
         <v>1.1750881316098707E-3</v>
       </c>
@@ -1721,25 +1817,25 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <f t="shared" si="7"/>
         <v>1200</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>1250</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>2</v>
       </c>
       <c r="F26">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="H26" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="7">
+      <c r="H26" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="5">
         <f t="shared" si="4"/>
         <v>1.1750881316098707E-3</v>
       </c>
@@ -1753,25 +1849,25 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <f t="shared" si="7"/>
         <v>1250</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>1300</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>1</v>
       </c>
       <c r="F27">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H27" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I27" s="7">
+      <c r="H27" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="5">
         <f t="shared" si="4"/>
         <v>5.8754406580493535E-4</v>
       </c>
@@ -1785,25 +1881,25 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <f t="shared" si="7"/>
         <v>1300</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>1350</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <v>2</v>
       </c>
       <c r="F28">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="H28" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I28" s="7">
+      <c r="H28" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="5">
         <f t="shared" si="4"/>
         <v>1.1750881316098707E-3</v>
       </c>
@@ -1817,25 +1913,25 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="A29" s="3">
         <f t="shared" si="7"/>
         <v>1400</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>1450</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <v>3</v>
       </c>
       <c r="F29">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H29" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I29" s="7">
+      <c r="H29" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="5">
         <f t="shared" si="4"/>
         <v>1.7626321974148062E-3</v>
       </c>
@@ -1849,25 +1945,25 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <f t="shared" si="7"/>
         <v>1500</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>1550</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="2">
         <v>2</v>
       </c>
       <c r="F30">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="H30" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I30" s="7">
+      <c r="H30" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="5">
         <f t="shared" si="4"/>
         <v>1.1750881316098707E-3</v>
       </c>
@@ -1881,25 +1977,25 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="A31" s="3">
         <f t="shared" si="7"/>
         <v>1950</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>2000</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="2">
         <v>1</v>
       </c>
       <c r="F31">
         <f>SUM(C31:C35)</f>
         <v>5</v>
       </c>
-      <c r="H31" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I31" s="7">
+      <c r="H31" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="5">
         <f t="shared" si="4"/>
         <v>2.9377203290246769E-3</v>
       </c>
@@ -1913,21 +2009,21 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="A32" s="3">
         <f t="shared" si="7"/>
         <v>2000</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>2050</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="2">
         <v>1</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H32" s="5">
         <f t="shared" ref="H32:H35" si="8">E32/E$36</f>
         <v>0</v>
       </c>
-      <c r="I32" s="7">
+      <c r="I32" s="5">
         <f t="shared" ref="I32:I35" si="9">F32/F$36</f>
         <v>0</v>
       </c>
@@ -1941,21 +2037,21 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <f t="shared" si="7"/>
         <v>2150</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>2200</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="2">
         <v>1</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H33" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="I33" s="7">
+      <c r="I33" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -1969,21 +2065,21 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="A34" s="3">
         <f t="shared" si="7"/>
         <v>2250</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>2300</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="2">
         <v>1</v>
       </c>
-      <c r="H34" s="7">
+      <c r="H34" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="I34" s="7">
+      <c r="I34" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -1997,21 +2093,21 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <f t="shared" si="7"/>
         <v>3850</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>3900</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="2">
         <v>1</v>
       </c>
-      <c r="H35" s="7">
+      <c r="H35" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="I35" s="7">
+      <c r="I35" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>

</xml_diff>